<commit_message>
EXPORT aggiunta gestione mancanti e aggiunta in DDT
</commit_message>
<xml_diff>
--- a/functions/export/src/1/F023588-M074Q115.xlsx
+++ b/functions/export/src/1/F023588-M074Q115.xlsx
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1236</v>
+        <v>6664</v>
       </c>
       <c r="F2"/>
     </row>
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>857</v>
+        <v>125</v>
       </c>
       <c r="F3"/>
     </row>
@@ -736,7 +736,7 @@
         <v>0.08</v>
       </c>
       <c r="F7">
-        <v>68.56</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -756,7 +756,7 @@
         <v>0.18</v>
       </c>
       <c r="F8">
-        <v>154.26</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -776,7 +776,7 @@
         <v>0.13</v>
       </c>
       <c r="F9">
-        <v>111.41</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -796,7 +796,7 @@
         <v>0.128</v>
       </c>
       <c r="F10">
-        <v>109.7</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -816,7 +816,7 @@
         <v>0.035</v>
       </c>
       <c r="F11">
-        <v>30.0</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -836,7 +836,7 @@
         <v>0.035</v>
       </c>
       <c r="F12">
-        <v>30.0</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -856,7 +856,7 @@
         <v>0.016</v>
       </c>
       <c r="F13">
-        <v>13.71</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -876,7 +876,7 @@
         <v>0.04</v>
       </c>
       <c r="F14">
-        <v>34.28</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -896,7 +896,7 @@
         <v>0.02</v>
       </c>
       <c r="F15">
-        <v>17.14</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -916,7 +916,7 @@
         <v>0.115</v>
       </c>
       <c r="F16">
-        <v>98.56</v>
+        <v>14.38</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -936,7 +936,7 @@
         <v>0.025</v>
       </c>
       <c r="F17">
-        <v>21.43</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -956,7 +956,7 @@
         <v>0.016</v>
       </c>
       <c r="F18">
-        <v>13.71</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -976,7 +976,7 @@
         <v>0.017</v>
       </c>
       <c r="F19">
-        <v>14.57</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -996,7 +996,7 @@
         <v>0.023</v>
       </c>
       <c r="F20">
-        <v>19.71</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1026,7 +1026,7 @@
         <v>14</v>
       </c>
       <c r="F22">
-        <v>11998.0</v>
+        <v>1750.0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1046,7 +1046,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>5999.0</v>
+        <v>875.0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1066,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <v>2571.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1086,7 +1086,7 @@
         <v>1.5</v>
       </c>
       <c r="F25">
-        <v>1285.5</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1106,7 +1106,7 @@
         <v>8</v>
       </c>
       <c r="F26">
-        <v>6856.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1126,7 +1126,7 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>3428.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1146,7 +1146,7 @@
         <v>0.014</v>
       </c>
       <c r="F28">
-        <v>12.0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1166,7 +1166,7 @@
         <v>0.001</v>
       </c>
       <c r="F29">
-        <v>0.86</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1186,7 +1186,7 @@
         <v>0.001</v>
       </c>
       <c r="F30">
-        <v>0.86</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1206,7 +1206,7 @@
         <v>0.3</v>
       </c>
       <c r="F31">
-        <v>257.1</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1226,7 +1226,7 @@
         <v>1.5</v>
       </c>
       <c r="F32">
-        <v>1285.5</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1246,7 +1246,7 @@
         <v>0.7</v>
       </c>
       <c r="F33">
-        <v>599.9</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1266,7 +1266,7 @@
         <v>0.2</v>
       </c>
       <c r="F34">
-        <v>171.4</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1286,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>857.0</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1306,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>857.0</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1326,7 +1326,7 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>20568.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1346,7 +1346,7 @@
         <v>0.01</v>
       </c>
       <c r="F38">
-        <v>8.57</v>
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>